<commit_message>
updated manuscript, results, and additional notes.
</commit_message>
<xml_diff>
--- a/graphs/summary_tables_phasing.xlsx
+++ b/graphs/summary_tables_phasing.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixrichter/Dropbox/PhD/longreadclustersequencing/graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24159D8-041D-9C40-9812-4F136A82ABC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64FC54-542F-7B42-92B1-4116CBAF5CBA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33160" yWindow="-4760" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{AEAEB604-9D60-6C48-A1CF-B878A0784EFA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{AEAEB604-9D60-6C48-A1CF-B878A0784EFA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Combined" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Phased_by_method" sheetId="3" r:id="rId1"/>
+    <sheet name="Indel_stats" sheetId="1" r:id="rId2"/>
+    <sheet name="Tables_cleaned" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>Homopolymer run</t>
   </si>
@@ -82,6 +83,21 @@
   </si>
   <si>
     <t>Meta-analysis p-values (Fisher's method)</t>
+  </si>
+  <si>
+    <t>Indel</t>
+  </si>
+  <si>
+    <t>SNV</t>
+  </si>
+  <si>
+    <t>Fraction phased</t>
+  </si>
+  <si>
+    <t>Unphased</t>
+  </si>
+  <si>
+    <t>Meta-analysis (Fisher's method)</t>
   </si>
 </sst>
 </file>
@@ -135,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -168,6 +184,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -483,11 +508,158 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D8F08F-C4F0-F444-8436-E5ED44B59C84}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>138</v>
+      </c>
+      <c r="D2">
+        <v>445</v>
+      </c>
+      <c r="E2">
+        <v>105</v>
+      </c>
+      <c r="F2" s="16">
+        <f>(C2+D2)/SUM(C2:E2)</f>
+        <v>0.84738372093023251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="16">
+        <f>(C3+D3)/SUM(C3:E3)</f>
+        <v>0.82758620689655171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>213</v>
+      </c>
+      <c r="E4">
+        <v>420</v>
+      </c>
+      <c r="F4" s="16">
+        <f>(C4+D4)/SUM(C4:E4)</f>
+        <v>0.38953488372093026</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>37</v>
+      </c>
+      <c r="F5" s="16">
+        <f>(C5+D5)/SUM(C5:E5)</f>
+        <v>0.3728813559322034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>1217</v>
+      </c>
+      <c r="D6">
+        <v>3945</v>
+      </c>
+      <c r="E6">
+        <v>16860</v>
+      </c>
+      <c r="F6" s="16">
+        <f>(C6+D6)/SUM(C6:E6)</f>
+        <v>0.23440196167468894</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>82</v>
+      </c>
+      <c r="D7">
+        <v>224</v>
+      </c>
+      <c r="E7">
+        <f>1535 - (C7+D7)</f>
+        <v>1229</v>
+      </c>
+      <c r="F7" s="16">
+        <f>(C7+D7)/SUM(C7:E7)</f>
+        <v>0.19934853420195439</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1372C1CD-FD4C-5F41-B06F-1BBB89E3AB8F}">
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B2:J10"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,12 +934,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF5525A-B9FE-6742-BCFE-1C9B553A4A4B}">
-  <dimension ref="A3:I25"/>
+  <dimension ref="A3:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A23" sqref="A23:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,9 +949,10 @@
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
@@ -788,7 +961,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="14"/>
       <c r="C4" s="13" t="s">
@@ -803,8 +976,24 @@
       <c r="F4" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="20"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="14" t="s">
         <v>5</v>
@@ -822,11 +1011,33 @@
         <v>23</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" ref="E5:F5" si="1">SUM(F6:F7)</f>
+        <f t="shared" ref="F5" si="1">SUM(F6:F7)</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="17"/>
+      <c r="P5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="14" t="s">
         <v>6</v>
@@ -844,8 +1055,38 @@
         <f>C6+D6+E6</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="14" t="s">
         <v>7</v>
@@ -863,8 +1104,41 @@
         <f>C7+D7+E7</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <v>6.0856707951746199E-2</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0.86736788684099098</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0.133383385772541</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.71335969264547505</v>
+      </c>
+      <c r="L7" s="16">
+        <v>8.7550553669692902E-2</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0.125225618898642</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0.109667832983845</v>
+      </c>
+      <c r="O7" s="16">
+        <v>5.4525301895685697E-2</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0.34973813914332302</v>
+      </c>
+      <c r="Q7" s="16">
+        <v>0.16518651223001099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
@@ -883,8 +1157,41 @@
       <c r="F8" s="7">
         <v>0.33561157256156698</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>-3.2170047922470897E-4</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0.99929628027471296</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.77485877477619203</v>
+      </c>
+      <c r="K8" s="5">
+        <v>8.4796244395013501E-3</v>
+      </c>
+      <c r="L8" s="16">
+        <v>4.2198123572786302E-2</v>
+      </c>
+      <c r="M8" s="16">
+        <v>0.460580321080792</v>
+      </c>
+      <c r="N8" s="18">
+        <v>0.14829816117226499</v>
+      </c>
+      <c r="O8" s="5">
+        <v>9.1481551941133502E-3</v>
+      </c>
+      <c r="P8" s="19">
+        <v>0.81740211977251798</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>8.1174570205311204E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="14" t="s">
         <v>15</v>
@@ -901,8 +1208,41 @@
       <c r="F9" s="7">
         <v>0.34310231278041903</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0.47313677835359202</v>
+      </c>
+      <c r="I9" s="16">
+        <v>0.16724291710431699</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0.142253808299002</v>
+      </c>
+      <c r="K9" s="16">
+        <v>0.69504079351735104</v>
+      </c>
+      <c r="L9" s="16">
+        <v>5.6423732716024001E-2</v>
+      </c>
+      <c r="M9" s="16">
+        <v>0.32364623511086699</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0.109102360129886</v>
+      </c>
+      <c r="O9" s="16">
+        <v>5.5790766080513497E-2</v>
+      </c>
+      <c r="P9" s="16">
+        <v>0.21198575750673801</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>0.16479899730564199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
@@ -921,8 +1261,41 @@
       <c r="F10" s="7">
         <v>0.73135156877178098</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="16">
+        <v>0.33561157256156698</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0.34310231278041903</v>
+      </c>
+      <c r="J10" s="18">
+        <v>0.73135156877178098</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1.6232754879015199E-2</v>
+      </c>
+      <c r="L10" s="16">
+        <v>8.5343078431225697E-2</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0.135070418423648</v>
+      </c>
+      <c r="N10" s="18">
+        <v>0.193160794779831</v>
+      </c>
+      <c r="O10" s="5">
+        <v>6.5362179627356397E-4</v>
+      </c>
+      <c r="P10" s="19">
+        <v>0.18869401593853499</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>1.32134845166831E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="14" t="s">
         <v>15</v>
@@ -940,11 +1313,11 @@
         <v>1.6232754879015199E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
@@ -963,7 +1336,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="12" t="s">
         <v>5</v>
@@ -985,7 +1358,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="12" t="s">
         <v>6</v>
@@ -1004,7 +1377,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="12" t="s">
         <v>7</v>
@@ -1165,6 +1538,15 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>